<commit_message>
copy row height on #each
</commit_message>
<xml_diff>
--- a/example/template.xlsx
+++ b/example/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishi/java/xlsx-template/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2944DA-D813-ED4E-A154-D7B890E3D2EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647B461-A359-C247-A706-08A0E8A1C19B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20340" yWindow="13520" windowWidth="38040" windowHeight="24280" xr2:uid="{CAB25370-319D-5847-9DA4-E8B4888F6D10}"/>
   </bookViews>
@@ -231,6 +231,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -241,9 +244,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +563,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -596,11 +596,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
@@ -610,12 +610,12 @@
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:5" ht="40" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -623,10 +623,10 @@
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
@@ -642,11 +642,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
@@ -656,12 +656,12 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" ht="40" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -669,10 +669,10 @@
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
@@ -685,11 +685,11 @@
         <v>3</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
@@ -699,12 +699,12 @@
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:5" ht="40" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -712,10 +712,10 @@
       <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">

</xml_diff>

<commit_message>
add image to example, update README
</commit_message>
<xml_diff>
--- a/example/template.xlsx
+++ b/example/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishi/java/xlsx-template/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647B461-A359-C247-A706-08A0E8A1C19B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7ABF26-D775-CB43-A358-523C437F25B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="13520" windowWidth="38040" windowHeight="24280" xr2:uid="{CAB25370-319D-5847-9DA4-E8B4888F6D10}"/>
+    <workbookView xWindow="8980" yWindow="12380" windowWidth="38040" windowHeight="24280" xr2:uid="{CAB25370-319D-5847-9DA4-E8B4888F6D10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,6 +261,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>59266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E3517BB-62E8-E345-9AE8-FDDE125A4374}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5626100" y="279399"/>
+          <a:ext cx="1549400" cy="2065867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,7 +612,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -745,5 +794,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
support merged cells covers added/removed row
</commit_message>
<xml_diff>
--- a/example/template.xlsx
+++ b/example/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishi/java/xlsx-template/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7ABF26-D775-CB43-A358-523C437F25B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6689D371-ADC3-4044-8C8B-D261F23FF1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="12380" windowWidth="38040" windowHeight="24280" xr2:uid="{CAB25370-319D-5847-9DA4-E8B4888F6D10}"/>
+    <workbookView xWindow="41400" yWindow="15300" windowWidth="38040" windowHeight="24280" xr2:uid="{CAB25370-319D-5847-9DA4-E8B4888F6D10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
   <si>
     <t>beforeRow</t>
     <phoneticPr fontId="1"/>
@@ -81,6 +81,46 @@
   </si>
   <si>
     <t>* Footer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>m5</t>
+  </si>
+  <si>
+    <t>m3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m1-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m2-3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m2-4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m3-4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m4-5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -125,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -185,13 +225,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,20 +377,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4F4B7F-CEF0-3B4C-AFC9-4E495A0DE37B}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -645,11 +839,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
@@ -659,10 +853,10 @@
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" ht="40" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -672,10 +866,10 @@
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
@@ -691,11 +885,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
@@ -705,10 +899,10 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5" ht="40" customHeight="1">
       <c r="A10" s="7" t="s">
@@ -718,10 +912,10 @@
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
@@ -734,11 +928,11 @@
         <v>3</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
@@ -748,10 +942,10 @@
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:5" ht="40" customHeight="1">
       <c r="A14" s="7" t="s">
@@ -761,10 +955,10 @@
       <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
@@ -776,21 +970,209 @@
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="C16" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="B18" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="8"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" s="8"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="C29" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
+  <mergeCells count="21">
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>